<commit_message>
finalized the gift presentation
</commit_message>
<xml_diff>
--- a/datascience_in_practice/finding_a_gift_using_data_science/data/wine_taste.xlsx
+++ b/datascience_in_practice/finding_a_gift_using_data_science/data/wine_taste.xlsx
@@ -15,8 +15,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Andreas Steffen</author>
+  </authors>
+  <commentList>
+    <comment ref="B22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andreas Steffen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+leave this open as we want to predict it</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andreas Steffen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -133,29 +191,63 @@
   </si>
   <si>
     <t>Georgina</t>
+  </si>
+  <si>
+    <t>Melanie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -163,14 +255,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,32 +574,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -798,7 +911,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -818,7 +931,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -838,7 +951,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -858,7 +971,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -878,7 +991,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -898,8 +1011,29 @@
         <v>36</v>
       </c>
     </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>